<commit_message>
19-01-2025 Vertical spritemoving added
</commit_message>
<xml_diff>
--- a/Suite system5/Doc/Spritedesigner.xlsx
+++ b/Suite system5/Doc/Spritedesigner.xlsx
@@ -26,6 +26,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>32,96,48,32,</t>
+  </si>
+  <si>
+    <t>32,111,33,32,</t>
+  </si>
+  <si>
+    <t>42,35,116,32</t>
+  </si>
+  <si>
+    <t>32,104,52,32,</t>
+  </si>
+  <si>
+    <t>32,127,112,32,</t>
+  </si>
+  <si>
+    <t>32,106,48,32</t>
+  </si>
+  <si>
+    <t>32,126,49,32,</t>
+  </si>
+  <si>
+    <t>104,38,45,32</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG29"/>
+  <dimension ref="A1:AG59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21:AG23"/>
+      <selection activeCell="A31" sqref="A31:H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,23 +1764,535 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="7"/>
     </row>
+    <row r="30" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="3"/>
+      <c r="J31">
+        <v>32</v>
+      </c>
+      <c r="K31">
+        <v>96</v>
+      </c>
+      <c r="L31">
+        <v>48</v>
+      </c>
+      <c r="M31">
+        <v>32</v>
+      </c>
+      <c r="O31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="O32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="7"/>
+      <c r="O33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="3"/>
+      <c r="J34">
+        <v>32</v>
+      </c>
+      <c r="K34">
+        <v>111</v>
+      </c>
+      <c r="L34">
+        <v>33</v>
+      </c>
+      <c r="M34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3"/>
+      <c r="J37">
+        <v>42</v>
+      </c>
+      <c r="K37">
+        <v>35</v>
+      </c>
+      <c r="L37">
+        <v>116</v>
+      </c>
+      <c r="M37">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="6">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="3"/>
+      <c r="J41">
+        <v>32</v>
+      </c>
+      <c r="K41">
+        <v>104</v>
+      </c>
+      <c r="L41">
+        <v>52</v>
+      </c>
+      <c r="M41">
+        <v>32</v>
+      </c>
+      <c r="O41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="5">
+        <v>1</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="5"/>
+      <c r="O42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="7">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="7"/>
+      <c r="O43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="3"/>
+      <c r="J44">
+        <v>32</v>
+      </c>
+      <c r="K44">
+        <v>127</v>
+      </c>
+      <c r="L44">
+        <v>112</v>
+      </c>
+      <c r="M44">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="6">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="3"/>
+      <c r="J47">
+        <v>32</v>
+      </c>
+      <c r="K47">
+        <v>106</v>
+      </c>
+      <c r="L47">
+        <v>48</v>
+      </c>
+      <c r="M47">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="5">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="7">
+        <v>1</v>
+      </c>
+      <c r="E49" s="6">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="3"/>
+      <c r="J51">
+        <v>32</v>
+      </c>
+      <c r="K51">
+        <v>96</v>
+      </c>
+      <c r="L51">
+        <v>48</v>
+      </c>
+      <c r="M51">
+        <v>32</v>
+      </c>
+      <c r="O51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="5"/>
+      <c r="O52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="7">
+        <v>1</v>
+      </c>
+      <c r="E53" s="6">
+        <v>1</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="7"/>
+      <c r="O53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="3"/>
+      <c r="J54">
+        <v>32</v>
+      </c>
+      <c r="K54">
+        <v>126</v>
+      </c>
+      <c r="L54">
+        <v>49</v>
+      </c>
+      <c r="M54">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="5">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="6">
+        <v>1</v>
+      </c>
+      <c r="D56" s="7">
+        <v>1</v>
+      </c>
+      <c r="E56" s="6">
+        <v>1</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="3"/>
+      <c r="J57">
+        <v>104</v>
+      </c>
+      <c r="K57">
+        <v>38</v>
+      </c>
+      <c r="L57">
+        <v>45</v>
+      </c>
+      <c r="M57">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5">
+        <v>1</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="4">
+        <v>1</v>
+      </c>
+      <c r="F58" s="5">
+        <v>1</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7">
+        <v>1</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A20:H29">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20:Z29">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:Z19">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H19">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:H59">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:H49">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
25-01-2025 Fixed DELAY command
</commit_message>
<xml_diff>
--- a/Suite system5/Doc/Spritedesigner.xlsx
+++ b/Suite system5/Doc/Spritedesigner.xlsx
@@ -29,32 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>32,96,48,32,</t>
-  </si>
-  <si>
-    <t>32,111,33,32,</t>
-  </si>
-  <si>
-    <t>42,35,116,32</t>
-  </si>
-  <si>
-    <t>32,104,52,32,</t>
-  </si>
-  <si>
-    <t>32,127,112,32,</t>
-  </si>
-  <si>
-    <t>32,106,48,32</t>
-  </si>
-  <si>
-    <t>32,126,49,32,</t>
-  </si>
-  <si>
-    <t>104,38,45,32</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -205,7 +180,42 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -564,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:H59"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O51" sqref="O51:O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,113 +594,101 @@
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="3">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3">
-        <v>1</v>
-      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
       <c r="J1">
         <f>1*A1+2*B1+4*A2+8*B2+16*A3+32+64*B3</f>
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="K1">
         <f>1*C1+2*D1+4*C2+8*D2+16*C3+32+64*D3</f>
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L1">
         <f>1*E1+2*F1+4*E2+8*F2+16*E3+32+64*F3</f>
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="M1">
         <f>1*G1+2*H1+4*G2+8*H2+16*G3+32+64*H3</f>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="O1" t="str">
         <f>CONCATENATE(J1,",",K1,",",L1,",",M1,"," )</f>
-        <v>32,102,127,32,</v>
+        <v>100,96,48,56,</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
       <c r="U1" s="2"/>
-      <c r="V1" s="3">
-        <v>1</v>
-      </c>
-      <c r="W1" s="2">
-        <v>1</v>
-      </c>
-      <c r="X1" s="3">
-        <v>1</v>
-      </c>
+      <c r="V1" s="3"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="3"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="3"/>
       <c r="AB1">
-        <f>1*S1+2*T1+4*S2+8*T2+16*S3+32+64*T3</f>
-        <v>32</v>
+        <f t="shared" ref="AB1" si="0">1*S1+2*T1+4*S2+8*T2+16*S3+32+64*T3</f>
+        <v>40</v>
       </c>
       <c r="AC1">
         <f>1*U1+2*V1+4*U2+8*V2+16*U3+32+64*V3</f>
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="AD1">
         <f>1*W1+2*X1+4*W2+8*X2+16*W3+32+64*X3</f>
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="AE1">
         <f>1*Y1+2*Z1+4*Y2+8*Z2+16*Y3+32+64*Z3</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AG1" t="str">
         <f>CONCATENATE(AB1,",",AC1,",",AD1,",",AE1,"," )</f>
-        <v>32,102,127,32,</v>
+        <v>40,52,96,36,</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
       <c r="O2" t="str">
         <f>CONCATENATE(J4,",",K4,",",L4,",",M4,"," )</f>
-        <v>32,112,125,32,</v>
+        <v>120,123,119,116,</v>
       </c>
       <c r="S2" s="4"/>
-      <c r="T2" s="5"/>
+      <c r="T2" s="5">
+        <v>1</v>
+      </c>
       <c r="U2" s="4">
         <v>1</v>
       </c>
       <c r="V2" s="5"/>
-      <c r="W2" s="4">
-        <v>1</v>
-      </c>
-      <c r="X2" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="4">
+        <v>1</v>
+      </c>
       <c r="Z2" s="5"/>
       <c r="AG2" t="str">
         <f>CONCATENATE(AB4,",",AC4,",",AD4,",",AE4,"," )</f>
-        <v>32,112,125,32,</v>
+        <v>44,52,104,44,</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7">
         <v>1</v>
@@ -698,24 +696,22 @@
       <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="O3" t="str">
         <f>CONCATENATE(J7,",",K7,",",L7,",",M7 )</f>
-        <v>32,96,127,32</v>
+        <v>41,112,112,38</v>
       </c>
       <c r="S3" s="6"/>
       <c r="T3" s="7"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="7">
-        <v>1</v>
-      </c>
-      <c r="W3" s="6">
-        <v>1</v>
-      </c>
+      <c r="U3" s="6">
+        <v>1</v>
+      </c>
+      <c r="V3" s="7"/>
+      <c r="W3" s="6"/>
       <c r="X3" s="7">
         <v>1</v>
       </c>
@@ -723,92 +719,112 @@
       <c r="Z3" s="7"/>
       <c r="AG3" t="str">
         <f>CONCATENATE(AB7,",",AC7,",",AD7,",",AE7 )</f>
-        <v>32,96,127,32</v>
+        <v>54,106,32,101</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
       <c r="J4">
         <f>1*A4+2*B4+4*A5+8*B5+16*A6+32+64*B6</f>
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="K4">
         <f>1*C4+2*D4+4*C5+8*D5+16*C6+32+64*D6</f>
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="L4">
         <f>1*E4+2*F4+4*E5+8*F5+16*E6+32+64*F6</f>
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="M4">
         <f>1*G4+2*H4+4*G5+8*H5+16*G6+32+64*H6</f>
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
       <c r="U4" s="2"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="2">
-        <v>1</v>
-      </c>
+      <c r="W4" s="2"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="3"/>
       <c r="AB4">
         <f>1*S4+2*T4+4*S5+8*T5+16*S6+32+64*T6</f>
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="AC4">
-        <f>1*U4+2*V4+4*U5+8*V5+16*U6+32+64*V6</f>
-        <v>112</v>
+        <f t="shared" ref="AC4" si="1">1*U4+2*V4+4*U5+8*V5+16*U6+32+64*V6</f>
+        <v>52</v>
       </c>
       <c r="AD4">
-        <f>1*W4+2*X4+4*W5+8*X5+16*W6+32+64*X6</f>
-        <v>125</v>
+        <f t="shared" ref="AD4" si="2">1*W4+2*X4+4*W5+8*X5+16*W6+32+64*X6</f>
+        <v>104</v>
       </c>
       <c r="AE4">
-        <f>1*Y4+2*Z4+4*Y5+8*Z5+16*Y6+32+64*Z6</f>
-        <v>32</v>
+        <f t="shared" ref="AE4" si="3">1*Y4+2*Z4+4*Y5+8*Z5+16*Y6+32+64*Z6</f>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
       <c r="H5" s="5"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="4"/>
+      <c r="S5" s="4">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4">
+        <v>1</v>
+      </c>
       <c r="V5" s="5"/>
-      <c r="W5" s="4">
-        <v>1</v>
-      </c>
+      <c r="W5" s="4"/>
       <c r="X5" s="5">
         <v>1</v>
       </c>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="5"/>
+      <c r="Y5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
       <c r="C6" s="6">
         <v>1</v>
       </c>
@@ -821,19 +837,19 @@
       <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
       <c r="S6" s="6"/>
       <c r="T6" s="7"/>
       <c r="U6" s="6">
         <v>1</v>
       </c>
-      <c r="V6" s="7">
-        <v>1</v>
-      </c>
-      <c r="W6" s="6">
-        <v>1</v>
-      </c>
+      <c r="V6" s="7"/>
+      <c r="W6" s="6"/>
       <c r="X6" s="7">
         <v>1</v>
       </c>
@@ -841,93 +857,99 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
       <c r="J7">
-        <f t="shared" ref="J7" si="0">1*A7+2*B7+4*A8+8*B8+16*A9+32+64*B9</f>
-        <v>32</v>
+        <f t="shared" ref="J7" si="4">1*A7+2*B7+4*A8+8*B8+16*A9+32+64*B9</f>
+        <v>41</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7" si="1">1*C7+2*D7+4*C8+8*D8+16*C9+32+64*D9</f>
-        <v>96</v>
+        <f t="shared" ref="K7" si="5">1*C7+2*D7+4*C8+8*D8+16*C9+32+64*D9</f>
+        <v>112</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7" si="2">1*E7+2*F7+4*E8+8*F8+16*E9+32+64*F9</f>
-        <v>127</v>
+        <f t="shared" ref="L7" si="6">1*E7+2*F7+4*E8+8*F8+16*E9+32+64*F9</f>
+        <v>112</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7" si="3">1*G7+2*H7+4*G8+8*H8+16*G9+32+64*H9</f>
-        <v>32</v>
+        <f t="shared" ref="M7" si="7">1*G7+2*H7+4*G8+8*H8+16*G9+32+64*H9</f>
+        <v>38</v>
       </c>
       <c r="S7" s="2"/>
-      <c r="T7" s="3"/>
+      <c r="T7" s="3">
+        <v>1</v>
+      </c>
       <c r="U7" s="2"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="2">
-        <v>1</v>
-      </c>
-      <c r="X7" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="2"/>
+      <c r="V7" s="3">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
       <c r="Z7" s="3"/>
       <c r="AB7">
-        <f t="shared" ref="AB7" si="4">1*S7+2*T7+4*S8+8*T8+16*S9+32+64*T9</f>
-        <v>32</v>
+        <f t="shared" ref="AB7" si="8">1*S7+2*T7+4*S8+8*T8+16*S9+32+64*T9</f>
+        <v>54</v>
       </c>
       <c r="AC7">
-        <f t="shared" ref="AC7" si="5">1*U7+2*V7+4*U8+8*V8+16*U9+32+64*V9</f>
-        <v>96</v>
+        <f t="shared" ref="AC7" si="9">1*U7+2*V7+4*U8+8*V8+16*U9+32+64*V9</f>
+        <v>106</v>
       </c>
       <c r="AD7">
-        <f t="shared" ref="AD7" si="6">1*W7+2*X7+4*W8+8*X8+16*W9+32+64*X9</f>
-        <v>127</v>
+        <f t="shared" ref="AD7" si="10">1*W7+2*X7+4*W8+8*X8+16*W9+32+64*X9</f>
+        <v>32</v>
       </c>
       <c r="AE7">
-        <f t="shared" ref="AE7" si="7">1*Y7+2*Z7+4*Y8+8*Z8+16*Y9+32+64*Z9</f>
-        <v>32</v>
+        <f t="shared" ref="AE7" si="11">1*Y7+2*Z7+4*Y8+8*Z8+16*Y9+32+64*Z9</f>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
       <c r="H8" s="5"/>
-      <c r="S8" s="4"/>
+      <c r="S8" s="4">
+        <v>1</v>
+      </c>
       <c r="T8" s="5"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="4">
-        <v>1</v>
-      </c>
-      <c r="X8" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="4"/>
+      <c r="V8" s="5">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
@@ -939,56 +961,50 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
-      <c r="S9" s="6"/>
+      <c r="S9" s="6">
+        <v>1</v>
+      </c>
       <c r="T9" s="7"/>
       <c r="U9" s="6"/>
       <c r="V9" s="7">
         <v>1</v>
       </c>
-      <c r="W9" s="6">
-        <v>1</v>
-      </c>
-      <c r="X9" s="7">
-        <v>1</v>
-      </c>
+      <c r="W9" s="6"/>
+      <c r="X9" s="7"/>
       <c r="Y9" s="6"/>
-      <c r="Z9" s="7"/>
+      <c r="Z9" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="J11">
-        <f t="shared" ref="J11" si="8">1*A11+2*B11+4*A12+8*B12+16*A13+32+64*B13</f>
-        <v>32</v>
+        <f t="shared" ref="J11" si="12">1*A11+2*B11+4*A12+8*B12+16*A13+32+64*B13</f>
+        <v>100</v>
       </c>
       <c r="K11">
         <f>1*C11+2*D11+4*C12+8*D12+16*C13+32+64*D13</f>
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L11">
         <f>1*E11+2*F11+4*E12+8*F12+16*E13+32+64*F13</f>
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="M11">
         <f>1*G11+2*H11+4*G12+8*H12+16*G13+32+64*H13</f>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="O11" t="str">
         <f>CONCATENATE(J11,",",K11,",",L11,",",M11,"," )</f>
-        <v>32,102,127,32,</v>
+        <v>100,96,48,56,</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="3"/>
@@ -1005,7 +1021,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="3"/>
       <c r="AB11">
-        <f t="shared" ref="AB11" si="9">1*S11+2*T11+4*S12+8*T12+16*S13+32+64*T13</f>
+        <f t="shared" ref="AB11" si="13">1*S11+2*T11+4*S12+8*T12+16*S13+32+64*T13</f>
         <v>32</v>
       </c>
       <c r="AC11">
@@ -1026,23 +1042,21 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
       <c r="O12" t="str">
         <f>CONCATENATE(J14,",",K14,",",L14,",",M14,"," )</f>
-        <v>32,112,125,32,</v>
+        <v>120,123,119,116,</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="5"/>
@@ -1065,7 +1079,9 @@
     </row>
     <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7">
         <v>1</v>
@@ -1073,14 +1089,14 @@
       <c r="E13" s="6">
         <v>1</v>
       </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="O13" t="str">
         <f>CONCATENATE(J17,",",K17,",",L17,",",M17 )</f>
-        <v>32,120,43,52</v>
+        <v>43,127,127,39</v>
       </c>
       <c r="S13" s="6"/>
       <c r="T13" s="7"/>
@@ -1104,29 +1120,35 @@
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="3"/>
       <c r="J14">
         <f>1*A14+2*B14+4*A15+8*B15+16*A16+32+64*B16</f>
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14" si="10">1*C14+2*D14+4*C15+8*D15+16*C16+32+64*D16</f>
-        <v>112</v>
+        <f t="shared" ref="K14" si="14">1*C14+2*D14+4*C15+8*D15+16*C16+32+64*D16</f>
+        <v>123</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14" si="11">1*E14+2*F14+4*E15+8*F15+16*E16+32+64*F16</f>
-        <v>125</v>
+        <f t="shared" ref="L14" si="15">1*E14+2*F14+4*E15+8*F15+16*E16+32+64*F16</f>
+        <v>119</v>
       </c>
       <c r="M14">
-        <f t="shared" ref="M14" si="12">1*G14+2*H14+4*G15+8*H15+16*G16+32+64*H16</f>
-        <v>32</v>
+        <f t="shared" ref="M14" si="16">1*G14+2*H14+4*G15+8*H15+16*G16+32+64*H16</f>
+        <v>116</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="3"/>
@@ -1143,30 +1165,34 @@
         <v>32</v>
       </c>
       <c r="AC14">
-        <f t="shared" ref="AC14" si="13">1*U14+2*V14+4*U15+8*V15+16*U16+32+64*V16</f>
+        <f t="shared" ref="AC14" si="17">1*U14+2*V14+4*U15+8*V15+16*U16+32+64*V16</f>
         <v>112</v>
       </c>
       <c r="AD14">
-        <f t="shared" ref="AD14" si="14">1*W14+2*X14+4*W15+8*X15+16*W16+32+64*X16</f>
+        <f t="shared" ref="AD14" si="18">1*W14+2*X14+4*W15+8*X15+16*W16+32+64*X16</f>
         <v>125</v>
       </c>
       <c r="AE14">
-        <f t="shared" ref="AE14" si="15">1*Y14+2*Z14+4*Y15+8*Z15+16*Y16+32+64*Z16</f>
+        <f t="shared" ref="AE14" si="19">1*Y14+2*Z14+4*Y15+8*Z15+16*Y16+32+64*Z16</f>
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="S15" s="4"/>
       <c r="T15" s="5"/>
@@ -1182,8 +1208,12 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
@@ -1196,8 +1226,12 @@
       <c r="F16" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1</v>
+      </c>
       <c r="S16" s="6"/>
       <c r="T16" s="7"/>
       <c r="U16" s="6">
@@ -1216,33 +1250,45 @@
       <c r="Z16" s="7"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
       <c r="J17">
-        <f t="shared" ref="J17" si="16">1*A17+2*B17+4*A18+8*B18+16*A19+32+64*B19</f>
-        <v>32</v>
+        <f t="shared" ref="J17" si="20">1*A17+2*B17+4*A18+8*B18+16*A19+32+64*B19</f>
+        <v>43</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17" si="17">1*C17+2*D17+4*C18+8*D18+16*C19+32+64*D19</f>
-        <v>120</v>
+        <f t="shared" ref="K17" si="21">1*C17+2*D17+4*C18+8*D18+16*C19+32+64*D19</f>
+        <v>127</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17" si="18">1*E17+2*F17+4*E18+8*F18+16*E19+32+64*F19</f>
-        <v>43</v>
+        <f t="shared" ref="L17" si="22">1*E17+2*F17+4*E18+8*F18+16*E19+32+64*F19</f>
+        <v>127</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17" si="19">1*G17+2*H17+4*G18+8*H18+16*G19+32+64*H19</f>
-        <v>52</v>
+        <f t="shared" ref="M17" si="23">1*G17+2*H17+4*G18+8*H18+16*G19+32+64*H19</f>
+        <v>39</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="3"/>
@@ -1257,30 +1303,36 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="3"/>
       <c r="AB17">
-        <f t="shared" ref="AB17" si="20">1*S17+2*T17+4*S18+8*T18+16*S19+32+64*T19</f>
+        <f t="shared" ref="AB17" si="24">1*S17+2*T17+4*S18+8*T18+16*S19+32+64*T19</f>
         <v>32</v>
       </c>
       <c r="AC17">
-        <f t="shared" ref="AC17" si="21">1*U17+2*V17+4*U18+8*V18+16*U19+32+64*V19</f>
+        <f t="shared" ref="AC17" si="25">1*U17+2*V17+4*U18+8*V18+16*U19+32+64*V19</f>
         <v>120</v>
       </c>
       <c r="AD17">
-        <f t="shared" ref="AD17" si="22">1*W17+2*X17+4*W18+8*X18+16*W19+32+64*X19</f>
+        <f t="shared" ref="AD17" si="26">1*W17+2*X17+4*W18+8*X18+16*W19+32+64*X19</f>
         <v>43</v>
       </c>
       <c r="AE17">
-        <f t="shared" ref="AE17" si="23">1*Y17+2*Z17+4*Y18+8*Z18+16*Y19+32+64*Z19</f>
+        <f t="shared" ref="AE17" si="27">1*Y17+2*Z17+4*Y18+8*Z18+16*Y19+32+64*Z19</f>
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
       <c r="D18" s="5">
         <v>1</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
       <c r="F18" s="5">
         <v>1</v>
       </c>
@@ -1312,11 +1364,13 @@
       <c r="D19" s="7">
         <v>1</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="6">
-        <v>1</v>
-      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="7"/>
       <c r="S19" s="6"/>
       <c r="T19" s="7"/>
@@ -1338,34 +1392,30 @@
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="3">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="3"/>
       <c r="G21" s="2"/>
       <c r="H21" s="3"/>
       <c r="J21">
-        <f t="shared" ref="J21" si="24">1*A21+2*B21+4*A22+8*B22+16*A23+32+64*B23</f>
-        <v>32</v>
+        <f t="shared" ref="J21" si="28">1*A21+2*B21+4*A22+8*B22+16*A23+32+64*B23</f>
+        <v>100</v>
       </c>
       <c r="K21">
         <f>1*C21+2*D21+4*C22+8*D22+16*C23+32+64*D23</f>
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="L21">
         <f>1*E21+2*F21+4*E22+8*F22+16*E23+32+64*F23</f>
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="M21">
         <f>1*G21+2*H21+4*G22+8*H22+16*G23+32+64*H23</f>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="O21" t="str">
         <f>CONCATENATE(J21,",",K21,",",L21,",",M21,"," )</f>
-        <v>32,54,105,32,</v>
+        <v>100,96,48,56,</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="3"/>
@@ -1384,7 +1434,7 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="3"/>
       <c r="AB21">
-        <f t="shared" ref="AB21" si="25">1*S21+2*T21+4*S22+8*T22+16*S23+32+64*T23</f>
+        <f t="shared" ref="AB21" si="29">1*S21+2*T21+4*S22+8*T22+16*S23+32+64*T23</f>
         <v>56</v>
       </c>
       <c r="AC21">
@@ -1405,21 +1455,21 @@
       </c>
     </row>
     <row r="22" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="5">
-        <v>1</v>
-      </c>
+      <c r="F22" s="5"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
       <c r="O22" t="str">
         <f>CONCATENATE(J24,",",K24,",",L24,",",M24,"," )</f>
-        <v>104,107,55,52,</v>
+        <v>120,123,119,116,</v>
       </c>
       <c r="S22" s="4"/>
       <c r="T22" s="5">
@@ -1446,20 +1496,24 @@
     </row>
     <row r="23" spans="1:33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6"/>
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
       <c r="H23" s="7"/>
       <c r="O23" t="str">
         <f>CONCATENATE(J27,",",K27,",",L27,",",M27 )</f>
-        <v>96,55,107,48</v>
+        <v>43,33,34,39</v>
       </c>
       <c r="S23" s="6">
         <v>1</v>
@@ -1507,19 +1561,19 @@
       <c r="H24" s="3"/>
       <c r="J24">
         <f>1*A24+2*B24+4*A25+8*B25+16*A26+32+64*B26</f>
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24" si="26">1*C24+2*D24+4*C25+8*D25+16*C26+32+64*D26</f>
-        <v>107</v>
+        <f t="shared" ref="K24" si="30">1*C24+2*D24+4*C25+8*D25+16*C26+32+64*D26</f>
+        <v>123</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24" si="27">1*E24+2*F24+4*E25+8*F25+16*E26+32+64*F26</f>
-        <v>55</v>
+        <f t="shared" ref="L24" si="31">1*E24+2*F24+4*E25+8*F25+16*E26+32+64*F26</f>
+        <v>119</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24" si="28">1*G24+2*H24+4*G25+8*H25+16*G26+32+64*H26</f>
-        <v>52</v>
+        <f t="shared" ref="M24" si="32">1*G24+2*H24+4*G25+8*H25+16*G26+32+64*H26</f>
+        <v>116</v>
       </c>
       <c r="S24" s="2">
         <v>1</v>
@@ -1548,15 +1602,15 @@
         <v>53</v>
       </c>
       <c r="AC24">
-        <f t="shared" ref="AC24" si="29">1*U24+2*V24+4*U25+8*V25+16*U26+32+64*V26</f>
+        <f t="shared" ref="AC24" si="33">1*U24+2*V24+4*U25+8*V25+16*U26+32+64*V26</f>
         <v>127</v>
       </c>
       <c r="AD24">
-        <f t="shared" ref="AD24" si="30">1*W24+2*X24+4*W25+8*X25+16*W26+32+64*X26</f>
+        <f t="shared" ref="AD24" si="34">1*W24+2*X24+4*W25+8*X25+16*W26+32+64*X26</f>
         <v>127</v>
       </c>
       <c r="AE24">
-        <f t="shared" ref="AE24" si="31">1*Y24+2*Z24+4*Y25+8*Z25+16*Y26+32+64*Z26</f>
+        <f t="shared" ref="AE24" si="35">1*Y24+2*Z24+4*Y25+8*Z25+16*Y26+32+64*Z26</f>
         <v>127</v>
       </c>
     </row>
@@ -1601,22 +1655,30 @@
       </c>
     </row>
     <row r="26" spans="1:33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6">
+        <v>1</v>
+      </c>
       <c r="B26" s="7">
         <v>1</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
       <c r="D26" s="7">
         <v>1</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
       <c r="G26" s="6">
         <v>1</v>
       </c>
-      <c r="H26" s="7"/>
+      <c r="H26" s="7">
+        <v>1</v>
+      </c>
       <c r="S26" s="6">
         <v>1</v>
       </c>
@@ -1641,37 +1703,41 @@
       </c>
     </row>
     <row r="27" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
-      <c r="D27" s="3">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="3">
         <v>1</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
       <c r="J27">
-        <f t="shared" ref="J27" si="32">1*A27+2*B27+4*A28+8*B28+16*A29+32+64*B29</f>
-        <v>96</v>
+        <f t="shared" ref="J27" si="36">1*A27+2*B27+4*A28+8*B28+16*A29+32+64*B29</f>
+        <v>43</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="K27" si="33">1*C27+2*D27+4*C28+8*D28+16*C29+32+64*D29</f>
-        <v>55</v>
+        <f t="shared" ref="K27" si="37">1*C27+2*D27+4*C28+8*D28+16*C29+32+64*D29</f>
+        <v>33</v>
       </c>
       <c r="L27">
-        <f t="shared" ref="L27" si="34">1*E27+2*F27+4*E28+8*F28+16*E29+32+64*F29</f>
-        <v>107</v>
+        <f t="shared" ref="L27" si="38">1*E27+2*F27+4*E28+8*F28+16*E29+32+64*F29</f>
+        <v>34</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27" si="35">1*G27+2*H27+4*G28+8*H28+16*G29+32+64*H29</f>
-        <v>48</v>
+        <f t="shared" ref="M27" si="39">1*G27+2*H27+4*G28+8*H28+16*G29+32+64*H29</f>
+        <v>39</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="3">
@@ -1692,34 +1758,34 @@
       </c>
       <c r="Z27" s="3"/>
       <c r="AB27">
-        <f t="shared" ref="AB27" si="36">1*S27+2*T27+4*S28+8*T28+16*S29+32+64*T29</f>
+        <f t="shared" ref="AB27" si="40">1*S27+2*T27+4*S28+8*T28+16*S29+32+64*T29</f>
         <v>34</v>
       </c>
       <c r="AC27">
-        <f t="shared" ref="AC27" si="37">1*U27+2*V27+4*U28+8*V28+16*U29+32+64*V29</f>
+        <f t="shared" ref="AC27" si="41">1*U27+2*V27+4*U28+8*V28+16*U29+32+64*V29</f>
         <v>46</v>
       </c>
       <c r="AD27">
-        <f t="shared" ref="AD27" si="38">1*W27+2*X27+4*W28+8*X28+16*W29+32+64*X29</f>
+        <f t="shared" ref="AD27" si="42">1*W27+2*X27+4*W28+8*X28+16*W29+32+64*X29</f>
         <v>47</v>
       </c>
       <c r="AE27">
-        <f t="shared" ref="AE27" si="39">1*Y27+2*Z27+4*Y28+8*Z28+16*Y29+32+64*Z29</f>
+        <f t="shared" ref="AE27" si="43">1*Y27+2*Z27+4*Y28+8*Z28+16*Y29+32+64*Z29</f>
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="5">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4">
+        <v>1</v>
+      </c>
       <c r="H28" s="5"/>
       <c r="S28" s="4"/>
       <c r="T28" s="5"/>
@@ -1740,20 +1806,12 @@
     </row>
     <row r="29" spans="1:33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="6">
-        <v>1</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="7"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="7">
-        <v>1</v>
-      </c>
-      <c r="G29" s="6">
-        <v>1</v>
-      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="7"/>
       <c r="S29" s="6"/>
       <c r="T29" s="7"/>
@@ -1775,37 +1833,49 @@
       <c r="G31" s="2"/>
       <c r="H31" s="3"/>
       <c r="J31">
-        <v>32</v>
+        <f t="shared" ref="J31" si="44">1*A31+2*B31+4*A32+8*B32+16*A33+32+64*B33</f>
+        <v>100</v>
       </c>
       <c r="K31">
+        <f>1*C31+2*D31+4*C32+8*D32+16*C33+32+64*D33</f>
         <v>96</v>
       </c>
       <c r="L31">
+        <f>1*E31+2*F31+4*E32+8*F32+16*E33+32+64*F33</f>
         <v>48</v>
       </c>
       <c r="M31">
-        <v>32</v>
-      </c>
-      <c r="O31" t="s">
-        <v>0</v>
+        <f>1*G31+2*H31+4*G32+8*H32+16*G33+32+64*H33</f>
+        <v>56</v>
+      </c>
+      <c r="O31" t="str">
+        <f>CONCATENATE(J31,",",K31,",",L31,",",M31,"," )</f>
+        <v>100,96,48,56,</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="4">
+        <v>1</v>
+      </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="5"/>
-      <c r="O32" t="s">
-        <v>1</v>
+      <c r="H32" s="5">
+        <v>1</v>
+      </c>
+      <c r="O32" t="str">
+        <f>CONCATENATE(J34,",",K34,",",L34,",",M34,"," )</f>
+        <v>120,123,119,116,</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
       <c r="C33" s="6"/>
       <c r="D33" s="7">
         <v>1</v>
@@ -1814,10 +1884,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
       <c r="H33" s="7"/>
-      <c r="O33" t="s">
-        <v>2</v>
+      <c r="O33" t="str">
+        <f>CONCATENATE(J37,",",K37,",",L37,",",M37 )</f>
+        <v>32,32,32,32</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -1832,86 +1905,104 @@
       <c r="E34" s="2">
         <v>1</v>
       </c>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="3"/>
       <c r="J34">
-        <v>32</v>
+        <f>1*A34+2*B34+4*A35+8*B35+16*A36+32+64*B36</f>
+        <v>120</v>
       </c>
       <c r="K34">
-        <v>111</v>
+        <f t="shared" ref="K34" si="45">1*C34+2*D34+4*C35+8*D35+16*C36+32+64*D36</f>
+        <v>123</v>
       </c>
       <c r="L34">
-        <v>33</v>
+        <f t="shared" ref="L34" si="46">1*E34+2*F34+4*E35+8*F35+16*E36+32+64*F36</f>
+        <v>119</v>
       </c>
       <c r="M34">
-        <v>32</v>
+        <f t="shared" ref="M34" si="47">1*G34+2*H34+4*G35+8*H35+16*G36+32+64*H36</f>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="4">
-        <v>1</v>
-      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>1</v>
+      </c>
       <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
+      <c r="A36" s="6">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
       <c r="D36" s="7">
         <v>1</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="7"/>
+      <c r="E36" s="6">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3">
-        <v>1</v>
-      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="3"/>
       <c r="J37">
-        <v>42</v>
+        <f t="shared" ref="J37" si="48">1*A37+2*B37+4*A38+8*B38+16*A39+32+64*B39</f>
+        <v>32</v>
       </c>
       <c r="K37">
-        <v>35</v>
+        <f t="shared" ref="K37" si="49">1*C37+2*D37+4*C38+8*D38+16*C39+32+64*D39</f>
+        <v>32</v>
       </c>
       <c r="L37">
-        <v>116</v>
+        <f t="shared" ref="L37" si="50">1*E37+2*F37+4*E38+8*F38+16*E39+32+64*F39</f>
+        <v>32</v>
       </c>
       <c r="M37">
+        <f t="shared" ref="M37" si="51">1*G37+2*H37+4*G38+8*H38+16*G39+32+64*H39</f>
         <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
+      <c r="B38" s="5"/>
       <c r="C38" s="4"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="4">
-        <v>1</v>
-      </c>
+      <c r="E38" s="4"/>
       <c r="F38" s="5"/>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -1921,12 +2012,8 @@
       <c r="B39" s="7"/>
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="6">
-        <v>1</v>
-      </c>
-      <c r="F39" s="7">
-        <v>1</v>
-      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="6"/>
       <c r="H39" s="7"/>
     </row>
@@ -1941,41 +2028,49 @@
       <c r="G41" s="2"/>
       <c r="H41" s="3"/>
       <c r="J41">
-        <v>32</v>
+        <f t="shared" ref="J41" si="52">1*A41+2*B41+4*A42+8*B42+16*A43+32+64*B43</f>
+        <v>100</v>
       </c>
       <c r="K41">
-        <v>104</v>
+        <f>1*C41+2*D41+4*C42+8*D42+16*C43+32+64*D43</f>
+        <v>96</v>
       </c>
       <c r="L41">
-        <v>52</v>
+        <f>1*E41+2*F41+4*E42+8*F42+16*E43+32+64*F43</f>
+        <v>48</v>
       </c>
       <c r="M41">
-        <v>32</v>
-      </c>
-      <c r="O41" t="s">
-        <v>3</v>
+        <f>1*G41+2*H41+4*G42+8*H42+16*G43+32+64*H43</f>
+        <v>56</v>
+      </c>
+      <c r="O41" t="str">
+        <f>CONCATENATE(J41,",",K41,",",L41,",",M41,"," )</f>
+        <v>100,96,48,56,</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="4">
+        <v>1</v>
+      </c>
       <c r="B42" s="5"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="5">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4">
-        <v>1</v>
-      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="5"/>
-      <c r="O42" t="s">
-        <v>4</v>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="O42" t="str">
+        <f>CONCATENATE(J44,",",K44,",",L44,",",M44,"," )</f>
+        <v>32,107,55,32,</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
+      <c r="B43" s="7">
+        <v>1</v>
+      </c>
       <c r="C43" s="6"/>
       <c r="D43" s="7">
         <v>1</v>
@@ -1984,10 +2079,13 @@
         <v>1</v>
       </c>
       <c r="F43" s="7"/>
-      <c r="G43" s="6"/>
+      <c r="G43" s="6">
+        <v>1</v>
+      </c>
       <c r="H43" s="7"/>
-      <c r="O43" t="s">
-        <v>5</v>
+      <c r="O43" t="str">
+        <f>CONCATENATE(J47,",",K47,",",L47,",",M47 )</f>
+        <v>32,32,32,32</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -1999,33 +2097,41 @@
       <c r="D44" s="3">
         <v>1</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="3"/>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="3"/>
       <c r="J44">
+        <f>1*A44+2*B44+4*A45+8*B45+16*A46+32+64*B46</f>
         <v>32</v>
       </c>
       <c r="K44">
-        <v>127</v>
+        <f t="shared" ref="K44" si="53">1*C44+2*D44+4*C45+8*D45+16*C46+32+64*D46</f>
+        <v>107</v>
       </c>
       <c r="L44">
-        <v>112</v>
+        <f t="shared" ref="L44" si="54">1*E44+2*F44+4*E45+8*F45+16*E46+32+64*F46</f>
+        <v>55</v>
       </c>
       <c r="M44">
+        <f t="shared" ref="M44" si="55">1*G44+2*H44+4*G45+8*H45+16*G46+32+64*H46</f>
         <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="4">
-        <v>1</v>
-      </c>
+      <c r="C45" s="4"/>
       <c r="D45" s="5">
         <v>1</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4">
+        <v>1</v>
+      </c>
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
@@ -2033,18 +2139,14 @@
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
-      <c r="C46" s="6">
-        <v>1</v>
-      </c>
+      <c r="C46" s="6"/>
       <c r="D46" s="7">
         <v>1</v>
       </c>
       <c r="E46" s="6">
         <v>1</v>
       </c>
-      <c r="F46" s="7">
-        <v>1</v>
-      </c>
+      <c r="F46" s="7"/>
       <c r="G46" s="6"/>
       <c r="H46" s="7"/>
     </row>
@@ -2052,23 +2154,25 @@
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="3">
-        <v>1</v>
-      </c>
+      <c r="D47" s="3"/>
       <c r="E47" s="2"/>
       <c r="F47" s="3"/>
       <c r="G47" s="2"/>
       <c r="H47" s="3"/>
       <c r="J47">
+        <f t="shared" ref="J47" si="56">1*A47+2*B47+4*A48+8*B48+16*A49+32+64*B49</f>
         <v>32</v>
       </c>
       <c r="K47">
-        <v>106</v>
+        <f t="shared" ref="K47" si="57">1*C47+2*D47+4*C48+8*D48+16*C49+32+64*D49</f>
+        <v>32</v>
       </c>
       <c r="L47">
-        <v>48</v>
+        <f t="shared" ref="L47" si="58">1*E47+2*F47+4*E48+8*F48+16*E49+32+64*F49</f>
+        <v>32</v>
       </c>
       <c r="M47">
+        <f t="shared" ref="M47" si="59">1*G47+2*H47+4*G48+8*H48+16*G49+32+64*H49</f>
         <v>32</v>
       </c>
     </row>
@@ -2076,9 +2180,7 @@
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="5">
-        <v>1</v>
-      </c>
+      <c r="D48" s="5"/>
       <c r="E48" s="4"/>
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
@@ -2088,12 +2190,8 @@
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="7">
-        <v>1</v>
-      </c>
-      <c r="E49" s="6">
-        <v>1</v>
-      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="7"/>
       <c r="G49" s="6"/>
       <c r="H49" s="7"/>
@@ -2109,19 +2207,24 @@
       <c r="G51" s="2"/>
       <c r="H51" s="3"/>
       <c r="J51">
+        <f t="shared" ref="J51" si="60">1*A51+2*B51+4*A52+8*B52+16*A53+32+64*B53</f>
         <v>32</v>
       </c>
       <c r="K51">
-        <v>96</v>
+        <f>1*C51+2*D51+4*C52+8*D52+16*C53+32+64*D53</f>
+        <v>32</v>
       </c>
       <c r="L51">
-        <v>48</v>
+        <f>1*E51+2*F51+4*E52+8*F52+16*E53+32+64*F53</f>
+        <v>32</v>
       </c>
       <c r="M51">
-        <v>32</v>
-      </c>
-      <c r="O51" t="s">
-        <v>0</v>
+        <f>1*G51+2*H51+4*G52+8*H52+16*G53+32+64*H53</f>
+        <v>32</v>
+      </c>
+      <c r="O51" t="str">
+        <f>CONCATENATE(J51,",",K51,",",L51,",",M51,"," )</f>
+        <v>32,32,32,32,</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -2133,25 +2236,23 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="5"/>
-      <c r="O52" t="s">
-        <v>6</v>
+      <c r="O52" t="str">
+        <f>CONCATENATE(J54,",",K54,",",L54,",",M54,"," )</f>
+        <v>32,42,37,32,</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="7"/>
       <c r="C53" s="6"/>
-      <c r="D53" s="7">
-        <v>1</v>
-      </c>
-      <c r="E53" s="6">
-        <v>1</v>
-      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="6"/>
       <c r="F53" s="7"/>
       <c r="G53" s="6"/>
       <c r="H53" s="7"/>
-      <c r="O53" t="s">
-        <v>7</v>
+      <c r="O53" t="str">
+        <f>CONCATENATE(J57,",",K57,",",L57,",",M57 )</f>
+        <v>32,32,32,32</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -2168,28 +2269,32 @@
       <c r="G54" s="2"/>
       <c r="H54" s="3"/>
       <c r="J54">
+        <f>1*A54+2*B54+4*A55+8*B55+16*A56+32+64*B56</f>
         <v>32</v>
       </c>
       <c r="K54">
-        <v>126</v>
+        <f t="shared" ref="K54" si="61">1*C54+2*D54+4*C55+8*D55+16*C56+32+64*D56</f>
+        <v>42</v>
       </c>
       <c r="L54">
-        <v>49</v>
+        <f t="shared" ref="L54" si="62">1*E54+2*F54+4*E55+8*F55+16*E56+32+64*F56</f>
+        <v>37</v>
       </c>
       <c r="M54">
+        <f t="shared" ref="M54" si="63">1*G54+2*H54+4*G55+8*H55+16*G56+32+64*H56</f>
         <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
-      <c r="C55" s="4">
-        <v>1</v>
-      </c>
+      <c r="C55" s="4"/>
       <c r="D55" s="5">
         <v>1</v>
       </c>
-      <c r="E55" s="4"/>
+      <c r="E55" s="4">
+        <v>1</v>
+      </c>
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="5"/>
@@ -2197,15 +2302,9 @@
     <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
-      <c r="C56" s="6">
-        <v>1</v>
-      </c>
-      <c r="D56" s="7">
-        <v>1</v>
-      </c>
-      <c r="E56" s="6">
-        <v>1</v>
-      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="7"/>
       <c r="G56" s="6"/>
       <c r="H56" s="7"/>
@@ -2214,51 +2313,41 @@
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="3">
-        <v>1</v>
-      </c>
-      <c r="E57" s="2">
-        <v>1</v>
-      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="2"/>
       <c r="F57" s="3"/>
       <c r="G57" s="2"/>
       <c r="H57" s="3"/>
       <c r="J57">
-        <v>104</v>
+        <f t="shared" ref="J57" si="64">1*A57+2*B57+4*A58+8*B58+16*A59+32+64*B59</f>
+        <v>32</v>
       </c>
       <c r="K57">
-        <v>38</v>
+        <f t="shared" ref="K57" si="65">1*C57+2*D57+4*C58+8*D58+16*C59+32+64*D59</f>
+        <v>32</v>
       </c>
       <c r="L57">
-        <v>45</v>
+        <f t="shared" ref="L57" si="66">1*E57+2*F57+4*E58+8*F58+16*E59+32+64*F59</f>
+        <v>32</v>
       </c>
       <c r="M57">
+        <f t="shared" ref="M57" si="67">1*G57+2*H57+4*G58+8*H58+16*G59+32+64*H59</f>
         <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="5">
-        <v>1</v>
-      </c>
-      <c r="C58" s="4">
-        <v>1</v>
-      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="4">
-        <v>1</v>
-      </c>
-      <c r="F58" s="5">
-        <v>1</v>
-      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="5"/>
       <c r="G58" s="4"/>
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
-      <c r="B59" s="7">
-        <v>1</v>
-      </c>
+      <c r="B59" s="7"/>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
       <c r="E59" s="6"/>
@@ -2267,32 +2356,52 @@
       <c r="H59" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A20:H29">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+  <conditionalFormatting sqref="A20:H20">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20:Z29">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:Z19">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H19">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:H59">
+  <conditionalFormatting sqref="A50:H50">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:H40">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:H29">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:H39">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:H49">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:H49">
+  <conditionalFormatting sqref="A51:H59">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
03-02-2025 DIGGING is working now
</commit_message>
<xml_diff>
--- a/Suite system5/Doc/Spritedesigner.xlsx
+++ b/Suite system5/Doc/Spritedesigner.xlsx
@@ -176,21 +176,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -669,7 +655,7 @@
   <dimension ref="A1:AG59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AG31" sqref="AG31:AG33"/>
+      <selection activeCell="O31" sqref="O31:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1050,7 @@
       </c>
       <c r="L11">
         <f>1*E11+2*F11+4*E12+8*F12+16*E13+32+64*F13</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M11">
         <f>1*G11+2*H11+4*G12+8*H12+16*G13+32+64*H13</f>
@@ -1072,7 +1058,7 @@
       </c>
       <c r="O11" t="str">
         <f>CONCATENATE(J11,",",K11,",",L11,",",M11,"," )</f>
-        <v>40,123,53,32,</v>
+        <v>40,123,57,32,</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="3"/>
@@ -1118,15 +1104,15 @@
       <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="O12" t="str">
         <f>CONCATENATE(J14,",",K14,",",L14,",",M14,"," )</f>
-        <v>96,58,52,32,</v>
+        <v>56,126,60,48,</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="5"/>
@@ -1164,7 +1150,7 @@
       <c r="H13" s="7"/>
       <c r="O13" t="str">
         <f>CONCATENATE(J17,",",K17,",",L17,",",M17 )</f>
-        <v>32,32,122,32</v>
+        <v>97,53,117,33</v>
       </c>
       <c r="S13" s="6"/>
       <c r="T13" s="7"/>
@@ -1198,19 +1184,19 @@
       <c r="H14" s="3"/>
       <c r="J14">
         <f>1*A14+2*B14+4*A15+8*B15+16*A16+32+64*B16</f>
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="K14">
         <f t="shared" ref="K14" si="14">1*C14+2*D14+4*C15+8*D15+16*C16+32+64*D16</f>
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="L14">
         <f t="shared" ref="L14" si="15">1*E14+2*F14+4*E15+8*F15+16*E16+32+64*F16</f>
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14" si="16">1*G14+2*H14+4*G15+8*H15+16*G16+32+64*H16</f>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="3"/>
@@ -1241,15 +1227,21 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
       <c r="S15" s="4"/>
@@ -1266,19 +1258,23 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7"/>
       <c r="C16" s="6">
         <v>1</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
       <c r="E16" s="6">
         <v>1</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="S16" s="6"/>
       <c r="T16" s="7"/>
@@ -1296,31 +1292,37 @@
       <c r="Z16" s="7"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2"/>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="J17">
         <f t="shared" ref="J17" si="20">1*A17+2*B17+4*A18+8*B18+16*A19+32+64*B19</f>
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="K17">
         <f t="shared" ref="K17" si="21">1*C17+2*D17+4*C18+8*D18+16*C19+32+64*D19</f>
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17" si="22">1*E17+2*F17+4*E18+8*F18+16*E19+32+64*F19</f>
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="M17">
         <f t="shared" ref="M17" si="23">1*G17+2*H17+4*G18+8*H18+16*G19+32+64*H19</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="3"/>
@@ -1352,12 +1354,14 @@
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5"/>
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
       <c r="S18" s="4"/>
@@ -1373,8 +1377,12 @@
     </row>
     <row r="19" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
       <c r="D19" s="7"/>
       <c r="E19" s="6">
         <v>1</v>
@@ -1423,7 +1431,7 @@
       </c>
       <c r="L21">
         <f>1*E21+2*F21+4*E22+8*F22+16*E23+32+64*F23</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M21">
         <f>1*G21+2*H21+4*G22+8*H22+16*G23+32+64*H23</f>
@@ -1431,7 +1439,7 @@
       </c>
       <c r="O21" t="str">
         <f>CONCATENATE(J21,",",K21,",",L21,",",M21,"," )</f>
-        <v>40,123,53,32,</v>
+        <v>40,123,57,32,</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="3"/>
@@ -1477,15 +1485,15 @@
       <c r="D22" s="4">
         <v>1</v>
       </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
       <c r="O22" t="str">
         <f>CONCATENATE(J24,",",K24,",",L24,",",M24,"," )</f>
-        <v>96,122,52,32,</v>
+        <v>56,126,60,48,</v>
       </c>
       <c r="S22" s="4"/>
       <c r="T22" s="5"/>
@@ -1523,7 +1531,7 @@
       <c r="H23" s="7"/>
       <c r="O23" t="str">
         <f>CONCATENATE(J27,",",K27,",",L27,",",M27 )</f>
-        <v>46,32,107,32</v>
+        <v>97,53,45,33</v>
       </c>
       <c r="S23" s="6"/>
       <c r="T23" s="7"/>
@@ -1557,19 +1565,19 @@
       <c r="H24" s="3"/>
       <c r="J24">
         <f>1*A24+2*B24+4*A25+8*B25+16*A26+32+64*B26</f>
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="K24">
         <f t="shared" ref="K24" si="30">1*C24+2*D24+4*C25+8*D25+16*C26+32+64*D26</f>
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="L24">
         <f t="shared" ref="L24" si="31">1*E24+2*F24+4*E25+8*F25+16*E26+32+64*F26</f>
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M24">
         <f t="shared" ref="M24" si="32">1*G24+2*H24+4*G25+8*H25+16*G26+32+64*H26</f>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="3"/>
@@ -1600,15 +1608,21 @@
     </row>
     <row r="25" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
       <c r="S25" s="4"/>
@@ -1625,10 +1639,10 @@
       <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:33" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
+      <c r="A26" s="6">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7"/>
       <c r="C26" s="6">
         <v>1</v>
       </c>
@@ -1639,7 +1653,9 @@
         <v>1</v>
       </c>
       <c r="F26" s="7"/>
-      <c r="G26" s="6"/>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
       <c r="H26" s="7"/>
       <c r="S26" s="6"/>
       <c r="T26" s="7"/>
@@ -1659,35 +1675,37 @@
       <c r="Z26" s="7"/>
     </row>
     <row r="27" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2"/>
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="2">
         <v>1</v>
       </c>
-      <c r="F27" s="3">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="J27">
         <f t="shared" ref="J27" si="36">1*A27+2*B27+4*A28+8*B28+16*A29+32+64*B29</f>
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="K27">
         <f t="shared" ref="K27" si="37">1*C27+2*D27+4*C28+8*D28+16*C29+32+64*D29</f>
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="L27">
         <f t="shared" ref="L27" si="38">1*E27+2*F27+4*E28+8*F28+16*E29+32+64*F29</f>
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="M27">
         <f t="shared" ref="M27" si="39">1*G27+2*H27+4*G28+8*H28+16*G29+32+64*H29</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="3"/>
@@ -1723,15 +1741,15 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>1</v>
-      </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
       <c r="F28" s="5">
         <v>1</v>
       </c>
@@ -1750,13 +1768,15 @@
     </row>
     <row r="29" spans="1:33" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1</v>
+      </c>
       <c r="D29" s="7"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="7">
-        <v>1</v>
-      </c>
+      <c r="F29" s="7"/>
       <c r="G29" s="6"/>
       <c r="H29" s="7"/>
       <c r="S29" s="6"/>
@@ -1796,7 +1816,7 @@
       </c>
       <c r="L31">
         <f>1*E31+2*F31+4*E32+8*F32+16*E33+32+64*F33</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M31">
         <f>1*G31+2*H31+4*G32+8*H32+16*G33+32+64*H33</f>
@@ -1804,7 +1824,7 @@
       </c>
       <c r="O31" t="str">
         <f>CONCATENATE(J31,",",K31,",",L31,",",M31,"," )</f>
-        <v>40,123,53,32,</v>
+        <v>40,123,57,32,</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="3"/>
@@ -1850,15 +1870,15 @@
       <c r="D32" s="4">
         <v>1</v>
       </c>
-      <c r="E32" s="5">
-        <v>1</v>
-      </c>
-      <c r="F32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
       <c r="O32" t="str">
         <f>CONCATENATE(J34,",",K34,",",L34,",",M34,"," )</f>
-        <v>32,122,52,32,</v>
+        <v>56,126,60,48,</v>
       </c>
       <c r="S32" s="4"/>
       <c r="T32" s="5"/>
@@ -1896,7 +1916,7 @@
       <c r="H33" s="7"/>
       <c r="O33" t="str">
         <f>CONCATENATE(J37,",",K37,",",L37,",",M37 )</f>
-        <v>96,53,33,32</v>
+        <v>41,37,117,33</v>
       </c>
       <c r="S33" s="6"/>
       <c r="T33" s="7"/>
@@ -1930,19 +1950,19 @@
       <c r="H34" s="3"/>
       <c r="J34">
         <f>1*A34+2*B34+4*A35+8*B35+16*A36+32+64*B36</f>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="K34">
         <f t="shared" ref="K34" si="46">1*C34+2*D34+4*C35+8*D35+16*C36+32+64*D36</f>
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="L34">
         <f t="shared" ref="L34" si="47">1*E34+2*F34+4*E35+8*F35+16*E36+32+64*F36</f>
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M34">
         <f t="shared" ref="M34" si="48">1*G34+2*H34+4*G35+8*H35+16*G36+32+64*H36</f>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="3"/>
@@ -1973,15 +1993,21 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
       <c r="D35" s="4">
         <v>1</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
       <c r="S35" s="4"/>
@@ -1998,7 +2024,9 @@
       <c r="Z35" s="5"/>
     </row>
     <row r="36" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
+      <c r="A36" s="6">
+        <v>1</v>
+      </c>
       <c r="B36" s="7"/>
       <c r="C36" s="6">
         <v>1</v>
@@ -2010,7 +2038,9 @@
         <v>1</v>
       </c>
       <c r="F36" s="7"/>
-      <c r="G36" s="6"/>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
       <c r="H36" s="7"/>
       <c r="S36" s="6"/>
       <c r="T36" s="7"/>
@@ -2028,7 +2058,9 @@
       <c r="Z36" s="7"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+      <c r="A37" s="2">
+        <v>1</v>
+      </c>
       <c r="B37" s="3"/>
       <c r="C37" s="2">
         <v>1</v>
@@ -2038,23 +2070,25 @@
         <v>1</v>
       </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2">
+        <v>1</v>
+      </c>
       <c r="H37" s="3"/>
       <c r="J37">
         <f t="shared" ref="J37" si="52">1*A37+2*B37+4*A38+8*B38+16*A39+32+64*B39</f>
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="K37">
         <f t="shared" ref="K37" si="53">1*C37+2*D37+4*C38+8*D38+16*C39+32+64*D39</f>
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="L37">
         <f t="shared" ref="L37" si="54">1*E37+2*F37+4*E38+8*F38+16*E39+32+64*F39</f>
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="M37">
         <f t="shared" ref="M37" si="55">1*G37+2*H37+4*G38+8*H38+16*G39+32+64*H39</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S37" s="2"/>
       <c r="T37" s="3"/>
@@ -2087,12 +2121,16 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
       <c r="C38" s="4">
         <v>1</v>
       </c>
       <c r="D38" s="5"/>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4">
+        <v>1</v>
+      </c>
       <c r="F38" s="5"/>
       <c r="G38" s="4"/>
       <c r="H38" s="5"/>
@@ -2109,15 +2147,15 @@
     </row>
     <row r="39" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
-      <c r="B39" s="7">
-        <v>1</v>
-      </c>
-      <c r="C39" s="6">
-        <v>1</v>
-      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="7"/>
+      <c r="E39" s="6">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
       <c r="G39" s="6"/>
       <c r="H39" s="7"/>
       <c r="S39" s="6"/>
@@ -2473,86 +2511,86 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A20:H20">
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20:Z20">
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:Z19">
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:H10 A16:H19 A11:A15 G11:H15 F1:H5">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:H50">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:H40">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:H49">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51:H59">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:F15">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A5">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:E5">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S21:Z29">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S31:Z39">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:H29 A21:A25 G21:H25">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:F25">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:H39 A31:A35 G31:H35">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:H49">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:H59">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:F15">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:F25">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:F35">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A5">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E5">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S21:Z29">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S31:Z39">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>